<commit_message>
[Assignment 3 ++] Compare performances of OpenMP static and MY static.
</commit_message>
<xml_diff>
--- a/assignment-3/experiment_data.xlsx
+++ b/assignment-3/experiment_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="11490" windowHeight="10800" activeTab="2"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="11490" windowHeight="10800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="p1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Serial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,6 +124,22 @@
   </si>
   <si>
     <t>thread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my static (1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my static (MAX)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size = 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max chunk size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -228,6 +244,9 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -249,14 +268,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1366,7 +1382,7 @@
   <autoFilter ref="B13:K15"/>
   <tableColumns count="10">
     <tableColumn id="1" name="thread"/>
-    <tableColumn id="2" name="1" dataDxfId="2">
+    <tableColumn id="2" name="1" dataDxfId="0">
       <calculatedColumnFormula>(C20+C21)/2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="2">
@@ -1413,8 +1429,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="표4" displayName="표4" ref="B6:F10" totalsRowShown="0">
-  <autoFilter ref="B6:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="표4" displayName="표4" ref="B6:F12" totalsRowShown="0">
+  <autoFilter ref="B6:F12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="thread"/>
     <tableColumn id="2" name="1"/>
@@ -2178,25 +2194,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F16"/>
+  <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="14.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -2213,7 +2232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -2230,83 +2249,120 @@
         <v>5.6826999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>6.3017000000000003</v>
+      </c>
+      <c r="E8">
+        <v>6.0128000000000004</v>
+      </c>
+      <c r="F8">
+        <v>6.5102000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>5.9861000000000004</v>
+      </c>
+      <c r="E9">
+        <v>5.6196000000000002</v>
+      </c>
+      <c r="F9">
+        <v>5.6618000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>8.3825000000000003</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>8.9271999999999991</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>8.0904000000000007</v>
       </c>
-      <c r="F8">
-        <v>11.676299999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="F10">
+        <v>8.2349999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>12.766</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>13.287599999999999</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>13.2379</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>13.239000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>8.4611000000000001</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>6.2309000000000001</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>5.8353000000000002</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <v>8.0239999999999991</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C13">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21">
         <v>6.0141</v>
       </c>
-      <c r="D13">
+      <c r="D21">
         <v>5.6845999999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22">
         <v>8.9271999999999991</v>
       </c>
-      <c r="D14">
+      <c r="D22">
         <v>11.616</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23">
         <v>13.287599999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C16">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24">
         <v>9.6725999999999992</v>
       </c>
-      <c r="D16">
+      <c r="D24">
         <v>8.0757999999999992</v>
       </c>
     </row>

</xml_diff>